<commit_message>
Updated staff data loader. Updated staff manager and inventory manager
</commit_message>
<xml_diff>
--- a/data/Staff_List.xlsx
+++ b/data/Staff_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Part Time Studies\OOP_Proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2E525C-6611-47FB-B335-3D5F9B26D38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40018992-A45C-4F6A-B088-739C5392924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Staff ID</t>
   </si>
@@ -37,18 +37,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>D001</t>
-  </si>
-  <si>
-    <t>D002</t>
-  </si>
-  <si>
-    <t>P001</t>
-  </si>
-  <si>
-    <t>A001</t>
-  </si>
-  <si>
     <t>Doctor</t>
   </si>
   <si>
@@ -76,43 +64,16 @@
     <t>Sarah Lee</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>DrJohnSmith</t>
-  </si>
-  <si>
-    <t>Pwd123</t>
-  </si>
-  <si>
-    <t>JohnSmith@testEmail.com</t>
-  </si>
-  <si>
-    <t>DrEmilyClarke</t>
-  </si>
-  <si>
-    <t>EmilyClarke@testEmail.com</t>
-  </si>
-  <si>
-    <t>PhMarkLee</t>
-  </si>
-  <si>
-    <t>MarkLee@testEmail.com</t>
-  </si>
-  <si>
-    <t>AdmSarahLee</t>
-  </si>
-  <si>
-    <t>SarahLee@testEmail.com</t>
-  </si>
-  <si>
-    <t>PhoneNo</t>
+    <t>S001</t>
+  </si>
+  <si>
+    <t>S002</t>
+  </si>
+  <si>
+    <t>S003</t>
+  </si>
+  <si>
+    <t>S004</t>
   </si>
 </sst>
 </file>
@@ -136,9 +97,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,22 +135,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,21 +447,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,143 +476,77 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2">
-        <v>12345678</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
       <c r="E3">
         <v>38</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>12345679</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <v>12345680</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5">
-        <v>12345681</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{C8F108FA-B1AD-4669-9489-72F141DD5175}"/>
-    <hyperlink ref="H3:H5" r:id="rId2" display="JohnSmith@testEmail.com" xr:uid="{84F17D34-B1F7-4141-ABB6-16F305B6432E}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{3727F3AD-4B11-459F-82E3-22A68A46DF45}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{18735CD6-F9E2-41E7-B0BA-9B9D9BEF6F98}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{A54691BA-FC8B-4216-9F81-C925652101C2}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>